<commit_message>
Fix create a course in Instructor dashboard
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED47D88-F891-4D5D-9425-3CFCD2DA441A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,31 +19,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
   <si>
-    <t>hello</t>
+    <t>SID</t>
   </si>
   <si>
-    <t>hiase</t>
+    <t>Name</t>
   </si>
   <si>
-    <t>asdfasf</t>
+    <t>S530742@nwmissouri.edu</t>
   </si>
   <si>
-    <t>asdfasfas</t>
-  </si>
-  <si>
-    <t>asrv</t>
+    <t>Naveen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -67,13 +71,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -351,46 +358,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A6" sqref="A6:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2"/>
+    <hyperlink ref="A4" r:id="rId3"/>
+    <hyperlink ref="A5" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Create button not showing is solved
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -1,42 +1,203 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531500\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA2AB7DD-16E8-43E5-B498-60DF3CA7A6C3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{AE42C86F-48A7-429A-A957-7E38505595EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
-  <si>
-    <t>SID</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>S530742@nwmissouri.edu</t>
-  </si>
-  <si>
-    <t>Naveen</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>Wellness</t>
+  </si>
+  <si>
+    <t>Whiskey</t>
+  </si>
+  <si>
+    <t>Witch</t>
+  </si>
+  <si>
+    <t>Would</t>
+  </si>
+  <si>
+    <t>Wound</t>
+  </si>
+  <si>
+    <t>Write</t>
+  </si>
+  <si>
+    <t>Wrong</t>
+  </si>
+  <si>
+    <t>Wrote</t>
+  </si>
+  <si>
+    <t>Xrayer</t>
+  </si>
+  <si>
+    <t>Yankee</t>
+  </si>
+  <si>
+    <t>Yesterday</t>
+  </si>
+  <si>
+    <t>Yield</t>
+  </si>
+  <si>
+    <t>Young</t>
+  </si>
+  <si>
+    <t>Zebra</t>
+  </si>
+  <si>
+    <t>Zombie</t>
+  </si>
+  <si>
+    <t>Zuluo</t>
+  </si>
+  <si>
+    <t>Pencil</t>
+  </si>
+  <si>
+    <t>Purple</t>
+  </si>
+  <si>
+    <t>Quasar</t>
+  </si>
+  <si>
+    <t>Quest</t>
+  </si>
+  <si>
+    <t>Quick</t>
+  </si>
+  <si>
+    <t>Redwood</t>
+  </si>
+  <si>
+    <t>Ringer</t>
+  </si>
+  <si>
+    <t>Romance</t>
+  </si>
+  <si>
+    <t>Rosea</t>
+  </si>
+  <si>
+    <t>Saturn</t>
+  </si>
+  <si>
+    <t>Sender</t>
+  </si>
+  <si>
+    <t>Shock</t>
+  </si>
+  <si>
+    <t>Shoot</t>
+  </si>
+  <si>
+    <t>Short</t>
+  </si>
+  <si>
+    <t>Shown</t>
+  </si>
+  <si>
+    <t>Sight</t>
+  </si>
+  <si>
+    <t>Since</t>
+  </si>
+  <si>
+    <t>Singer</t>
+  </si>
+  <si>
+    <t>Sixth</t>
+  </si>
+  <si>
+    <t>Sixty</t>
+  </si>
+  <si>
+    <t>Sized</t>
+  </si>
+  <si>
+    <t>Skill</t>
+  </si>
+  <si>
+    <t>Sleep</t>
+  </si>
+  <si>
+    <t>Slide</t>
+  </si>
+  <si>
+    <t>Small</t>
+  </si>
+  <si>
+    <t>Smart</t>
+  </si>
+  <si>
+    <t>Smile</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Steam</t>
+  </si>
+  <si>
+    <t>Steel</t>
+  </si>
+  <si>
+    <t>Steve</t>
+  </si>
+  <si>
+    <t>Stick</t>
+  </si>
+  <si>
+    <t>Still</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>Stone</t>
+  </si>
+  <si>
+    <t>Stood</t>
+  </si>
+  <si>
+    <t>Store</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -46,12 +207,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -71,16 +230,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -113,7 +270,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -125,7 +282,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -172,6 +329,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -207,6 +381,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -358,71 +549,289 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21C00EC2-BEAA-457B-BC9C-73991B0933F1}">
+  <dimension ref="A1:A54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+    </row>
+    <row r="2" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="4" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A8" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A24" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A26" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A27" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A30" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A32" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A33" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A34" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A35" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A36" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A37" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A38" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A39" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A40" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A41" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A42" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A43" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A44" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A45" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A46" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A47" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A48" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A49" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A50" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A51" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A52" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A53" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A54" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fetching proper course student details
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -1,54 +1,48 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531384\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689CDDF3-1D00-4B85-B460-6B23542ED8A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3570" xr2:uid="{27EC311A-257A-4E1E-9A20-7C1CC632166D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>SID</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>S530742@nwmissouri.edu</t>
-  </si>
-  <si>
-    <t>Naveen</t>
+    <t>Heklp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -71,16 +65,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -113,7 +104,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -125,7 +116,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -172,6 +163,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -207,6 +215,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -358,71 +383,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719BE7EC-7D77-43A9-B2B4-CEB6A9B4F1F8}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
-    <hyperlink ref="A5" r:id="rId4"/>
-    <hyperlink ref="A6" r:id="rId5"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fetching courses of student
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531384\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="B:\GDP2\Codeword-GDPII\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689CDDF3-1D00-4B85-B460-6B23542ED8A3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEC90609-AF27-445D-8BC0-EBC043F12932}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="3570" xr2:uid="{27EC311A-257A-4E1E-9A20-7C1CC632166D}"/>
   </bookViews>
@@ -30,19 +30,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
   <si>
-    <t>Heklp</t>
+    <t>S530742@nwmissouri.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Naveen </t>
+  </si>
+  <si>
+    <t>SID</t>
+  </si>
+  <si>
+    <t>Name</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -65,13 +82,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -384,18 +404,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{719BE7EC-7D77-43A9-B2B4-CEB6A9B4F1F8}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{36C8502F-BC8F-4ED9-A6AF-71C4B4A7CC6A}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{B15D2167-36EE-43E3-8B77-C3777996E8FC}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{F0097B7A-0E53-409E-90C1-B042FB82BE21}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{2ECAA5DD-8FB3-4EB8-A6A5-458B72F11BAF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modified active and inactive courses
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -1,111 +1,319 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s531383\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B53FCD5F-FC3E-422A-91C8-F7CE9F741C61}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{D1DE41AF-6572-4995-B021-87845475340D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>UDFHISH</t>
-  </si>
-  <si>
-    <t>FHISDG</t>
-  </si>
-  <si>
-    <t>FIKAHIO</t>
-  </si>
-  <si>
-    <t>GFIKFJ</t>
-  </si>
-  <si>
-    <t>VDJFUDIS</t>
-  </si>
-  <si>
-    <t>HDFGAIU</t>
-  </si>
-  <si>
-    <t>HCUkHFHFG</t>
-  </si>
-  <si>
-    <t>JDFGHUG</t>
-  </si>
-  <si>
-    <t>JFVHDGUF</t>
-  </si>
-  <si>
-    <t>SFUFGU</t>
-  </si>
-  <si>
-    <t>JFSFGGUFGU</t>
-  </si>
-  <si>
-    <t>SJHFUIAGUI</t>
-  </si>
-  <si>
-    <t>SFHDFISGU</t>
-  </si>
-  <si>
-    <t>FXFXNMFFSH</t>
-  </si>
-  <si>
-    <t>SNFJHUEGUG</t>
-  </si>
-  <si>
-    <t>MSDNJKAFHUA</t>
-  </si>
-  <si>
-    <t>NFVBUEGG</t>
-  </si>
-  <si>
-    <t>NJHGUHGU</t>
-  </si>
-  <si>
-    <t>FJSGHSU</t>
-  </si>
-  <si>
-    <t>GJUGESGU</t>
-  </si>
-  <si>
-    <t>ZJFIEUGUG</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+  <si>
+    <t>AFRICA</t>
+  </si>
+  <si>
+    <t>ALMOND</t>
+  </si>
+  <si>
+    <t>ANGER</t>
+  </si>
+  <si>
+    <t>AMERICA</t>
+  </si>
+  <si>
+    <t>BRAVO</t>
+  </si>
+  <si>
+    <t>BANKING</t>
+  </si>
+  <si>
+    <t>BOUNCE</t>
+  </si>
+  <si>
+    <t>BIGGER</t>
+  </si>
+  <si>
+    <t>COMPUTER</t>
+  </si>
+  <si>
+    <t>CANCER</t>
+  </si>
+  <si>
+    <t>CHAIR</t>
+  </si>
+  <si>
+    <t>CENTER</t>
+  </si>
+  <si>
+    <t>DAGGER</t>
+  </si>
+  <si>
+    <t>DESKS</t>
+  </si>
+  <si>
+    <t>DUMPED</t>
+  </si>
+  <si>
+    <t>BLACKDOG</t>
+  </si>
+  <si>
+    <t>ECHOES</t>
+  </si>
+  <si>
+    <t>ELVIS</t>
+  </si>
+  <si>
+    <t>EXTRA</t>
+  </si>
+  <si>
+    <t>ENGAGE</t>
+  </si>
+  <si>
+    <t>FRANCE</t>
+  </si>
+  <si>
+    <t>FOXTROT</t>
+  </si>
+  <si>
+    <t>FANCY</t>
+  </si>
+  <si>
+    <t>FELINE</t>
+  </si>
+  <si>
+    <t>GULFES</t>
+  </si>
+  <si>
+    <t>GINGER</t>
+  </si>
+  <si>
+    <t>GLOBE</t>
+  </si>
+  <si>
+    <t>GERMANY</t>
+  </si>
+  <si>
+    <t>HOTEL</t>
+  </si>
+  <si>
+    <t>HANGER</t>
+  </si>
+  <si>
+    <t>HELMET</t>
+  </si>
+  <si>
+    <t>HIDDEN</t>
+  </si>
+  <si>
+    <t>ICEBURG</t>
+  </si>
+  <si>
+    <t>INKSPOT</t>
+  </si>
+  <si>
+    <t>IMPULSE</t>
+  </si>
+  <si>
+    <t>IGORANCE</t>
+  </si>
+  <si>
+    <t>KILOMETERS</t>
+  </si>
+  <si>
+    <t>KANGAROO</t>
+  </si>
+  <si>
+    <t>KENNEDY</t>
+  </si>
+  <si>
+    <t>LEMONS</t>
+  </si>
+  <si>
+    <t>LINCON</t>
+  </si>
+  <si>
+    <t>LONDON</t>
+  </si>
+  <si>
+    <t>LINNER</t>
+  </si>
+  <si>
+    <t>MONKEY</t>
+  </si>
+  <si>
+    <t>MUMBAI</t>
+  </si>
+  <si>
+    <t>MONEY</t>
+  </si>
+  <si>
+    <t>MARKET</t>
+  </si>
+  <si>
+    <t>NATIVE</t>
+  </si>
+  <si>
+    <t>NUMBER</t>
+  </si>
+  <si>
+    <t>NOVEMBER</t>
+  </si>
+  <si>
+    <t>NICKEL</t>
+  </si>
+  <si>
+    <t>OBJECT</t>
+  </si>
+  <si>
+    <t>OPTION</t>
+  </si>
+  <si>
+    <t>OLDLIFE</t>
+  </si>
+  <si>
+    <t>OLIOCOOK</t>
+  </si>
+  <si>
+    <t>PICTURES</t>
+  </si>
+  <si>
+    <t>PENCIL</t>
+  </si>
+  <si>
+    <t>PURPLE</t>
+  </si>
+  <si>
+    <t>PUMPKIN</t>
+  </si>
+  <si>
+    <t>QUICKLY</t>
+  </si>
+  <si>
+    <t>QUASAR</t>
+  </si>
+  <si>
+    <t>QUALITY</t>
+  </si>
+  <si>
+    <t>ROMANCE</t>
+  </si>
+  <si>
+    <t>REDWOOD</t>
+  </si>
+  <si>
+    <t>RUSSIAN</t>
+  </si>
+  <si>
+    <t>RETIREMENT</t>
+  </si>
+  <si>
+    <t>STEVE</t>
+  </si>
+  <si>
+    <t>SENDER</t>
+  </si>
+  <si>
+    <t>SATURN</t>
+  </si>
+  <si>
+    <t>SINGER</t>
+  </si>
+  <si>
+    <t>TWILIGHT</t>
+  </si>
+  <si>
+    <t>TITANIC</t>
+  </si>
+  <si>
+    <t>TOWER</t>
+  </si>
+  <si>
+    <t>TALENT</t>
+  </si>
+  <si>
+    <t>UNIFORM</t>
+  </si>
+  <si>
+    <t>ULTIMATE</t>
+  </si>
+  <si>
+    <t>VICTORY</t>
+  </si>
+  <si>
+    <t>VAGRANT</t>
+  </si>
+  <si>
+    <t>VELVET</t>
+  </si>
+  <si>
+    <t>VOICE</t>
+  </si>
+  <si>
+    <t>WHISKEY</t>
+  </si>
+  <si>
+    <t>WITCH</t>
+  </si>
+  <si>
+    <t>WATER</t>
+  </si>
+  <si>
+    <t>WARNING</t>
+  </si>
+  <si>
+    <t>XEROXED</t>
+  </si>
+  <si>
+    <t>YANKEE</t>
+  </si>
+  <si>
+    <t>YESTERDAY</t>
+  </si>
+  <si>
+    <t>YOUNG</t>
+  </si>
+  <si>
+    <t>ZIPPED</t>
+  </si>
+  <si>
+    <t>ZINGER</t>
+  </si>
+  <si>
+    <t>ZOMBIE</t>
+  </si>
+  <si>
+    <t>ZEBRA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -128,8 +336,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -164,7 +375,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -176,7 +387,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -223,23 +434,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -275,23 +469,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -443,118 +620,473 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D634D688-3C4F-4035-8470-5BDD59F2ADCD}">
-  <dimension ref="A1:A21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection sqref="A1:A92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A88" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A89" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A90" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A91" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixes issues duplicate codewords
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531384\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S530742\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B180DC64-CD99-4A18-843F-2724547679DB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B043B6F5-E8B7-4867-8D63-427C8926945C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6645" xr2:uid="{1600F7D5-305A-44F7-BD75-E7962F1BB6D4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{79304DE6-FF10-4F3E-9807-C28912453DA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,46 +30,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
-  <si>
-    <t xml:space="preserve">above </t>
-  </si>
-  <si>
-    <t>frozen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fancy </t>
-  </si>
-  <si>
-    <t xml:space="preserve">hello </t>
-  </si>
-  <si>
-    <t>yummy</t>
-  </si>
-  <si>
-    <t>zombie</t>
-  </si>
-  <si>
-    <t>apple</t>
-  </si>
-  <si>
-    <t>elephant</t>
-  </si>
-  <si>
-    <t>banana</t>
-  </si>
-  <si>
-    <t>coconut</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>SGFAYTDSF</t>
+  </si>
+  <si>
+    <t>VCAGYFT</t>
+  </si>
+  <si>
+    <t>BVCHGFA</t>
+  </si>
+  <si>
+    <t>SDVAY@#HG</t>
+  </si>
+  <si>
+    <t>BVSH%&amp;*DBNVDHJ</t>
+  </si>
+  <si>
+    <t>BVSDHG</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -92,16 +88,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -413,11 +409,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{819A3EB0-11AB-4AB4-8206-C06F428B9459}">
-  <dimension ref="A1:A11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1824BFF-1CD6-472E-A1E7-A277624C3FE5}">
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,57 +424,34 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
+      <c r="A2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>8</v>
+      <c r="A4" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" xr:uid="{09FC8B74-0FF5-4FE0-BD13-DF9E75DC1E60}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixes issues in the course student
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -1,79 +1,60 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{054504EE-34FB-47AA-9645-3FA619695931}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531500\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BFCF38B8-CD38-4C11-B0E7-E1C510792738}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{E41FB720-665D-474E-95EA-BA568D94656E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>RANDOM</t>
+    <t>ABCDFSDF</t>
   </si>
   <si>
-    <t>CODEWORD</t>
+    <t>VDAG$%^</t>
   </si>
   <si>
-    <t>DUPLICATE</t>
+    <t>HCSYFGDY</t>
   </si>
   <si>
-    <t>SMALLER</t>
+    <t>VSHGDHDDH</t>
   </si>
   <si>
-    <t>TALLERS</t>
-  </si>
-  <si>
-    <t>IPHONES</t>
-  </si>
-  <si>
-    <t>MOBILES</t>
-  </si>
-  <si>
-    <t>TEMPERATURE</t>
-  </si>
-  <si>
-    <t>SNOW  ING</t>
-  </si>
-  <si>
-    <t>FA  ILURE</t>
+    <t>BVSHVDGH</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -96,17 +77,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -139,7 +116,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -151,7 +128,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -198,6 +175,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -233,6 +227,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -384,69 +395,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDE50FBC-9526-48BF-B0CD-E686387A005C}">
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes in the codeword set
</commit_message>
<xml_diff>
--- a/data/test.xlsx
+++ b/data/test.xlsx
@@ -1,60 +1,55 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S531500\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BFCF38B8-CD38-4C11-B0E7-E1C510792738}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC15208-FF67-44DC-BB06-456E383A252F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{E41FB720-665D-474E-95EA-BA568D94656E}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>ABCDFSDF</t>
+    <t>RANDOM</t>
   </si>
   <si>
-    <t>VDAG$%^</t>
-  </si>
-  <si>
-    <t>HCSYFGDY</t>
-  </si>
-  <si>
-    <t>VSHGDHDDH</t>
-  </si>
-  <si>
-    <t>BVSHVDGH</t>
+    <t>CODEWORD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -77,13 +72,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -116,7 +115,7 @@
         <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
         <a:srgbClr val="ED7D31"/>
@@ -128,7 +127,7 @@
         <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
         <a:srgbClr val="70AD47"/>
@@ -175,23 +174,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -227,23 +209,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -395,41 +360,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDE50FBC-9526-48BF-B0CD-E686387A005C}">
-  <dimension ref="A1:A5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="1"/>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
+      <c r="B2" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>